<commit_message>
Include first name of each athlete in 1000K race results.
</commit_message>
<xml_diff>
--- a/docs/RESULTS 1000KM_12th ULTRAMARATHON  FESTIVAL.xlsx
+++ b/docs/RESULTS 1000KM_12th ULTRAMARATHON  FESTIVAL.xlsx
@@ -57,19 +57,19 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>HOKIA</t>
-  </si>
-  <si>
-    <t>JAROSLAV</t>
-  </si>
-  <si>
-    <t>SANDOR</t>
-  </si>
-  <si>
     <t>RESULTS 1000KM</t>
   </si>
   <si>
     <t>NOT FINISHED</t>
+  </si>
+  <si>
+    <t>HOKIA LINTITA</t>
+  </si>
+  <si>
+    <t>SANDOR BOGI</t>
+  </si>
+  <si>
+    <t>JAROSLAV PRUCKNER</t>
   </si>
 </sst>
 </file>
@@ -181,10 +181,10 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -482,35 +482,35 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="6.7109375" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -552,14 +552,14 @@
       <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4">
         <v>100</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5">
         <v>115</v>
@@ -594,8 +594,8 @@
       <c r="M3" s="10">
         <v>743.45</v>
       </c>
-      <c r="N3" s="12" t="s">
-        <v>17</v>
+      <c r="N3" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -603,7 +603,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5">
         <v>104</v>
@@ -638,8 +638,8 @@
       <c r="M4" s="10">
         <v>754.65</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>17</v>
+      <c r="N4" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -647,7 +647,7 @@
         <v>102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5">
         <v>148</v>
@@ -682,8 +682,8 @@
       <c r="M5" s="3">
         <v>838</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>17</v>
+      <c r="N5" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include more details in 1000K race results.
</commit_message>
<xml_diff>
--- a/docs/RESULTS 1000KM_12th ULTRAMARATHON  FESTIVAL.xlsx
+++ b/docs/RESULTS 1000KM_12th ULTRAMARATHON  FESTIVAL.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Φύλλο2" sheetId="2" r:id="rId2"/>
     <sheet name="Φύλλο3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>BIB</t>
   </si>
@@ -54,9 +54,6 @@
     <t>10-day</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>RESULTS 1000KM</t>
   </si>
   <si>
@@ -70,6 +67,54 @@
   </si>
   <si>
     <t>JAROSLAV PRUCKNER</t>
+  </si>
+  <si>
+    <t>ALB</t>
+  </si>
+  <si>
+    <t>CZE</t>
+  </si>
+  <si>
+    <t>SVK</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>GRE</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>ALIMONTI DANIELE</t>
+  </si>
+  <si>
+    <t>MARIFOGLOU DIMOSTHENIS</t>
+  </si>
+  <si>
+    <t>1000miles split</t>
+  </si>
+  <si>
+    <t>TOTAL KM</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>9days 6hours 15min 54sec</t>
+  </si>
+  <si>
+    <t>9days 22hours 38min 00sec</t>
+  </si>
+  <si>
+    <t>10days</t>
+  </si>
+  <si>
+    <t>TOTAL TIME</t>
   </si>
 </sst>
 </file>
@@ -79,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,27 +134,29 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -121,7 +168,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,41 +200,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="46" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -195,7 +254,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -479,217 +538,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="6.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" s="13" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="11">
+        <v>6</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="12">
+        <v>141</v>
+      </c>
+      <c r="F3" s="12">
+        <v>112</v>
+      </c>
+      <c r="G3" s="12">
+        <v>104</v>
+      </c>
+      <c r="H3" s="12">
+        <v>118</v>
+      </c>
+      <c r="I3" s="12">
+        <v>101</v>
+      </c>
+      <c r="J3" s="12">
+        <v>98</v>
+      </c>
+      <c r="K3" s="12">
+        <v>111</v>
+      </c>
+      <c r="L3" s="12">
+        <v>92</v>
+      </c>
+      <c r="M3" s="12">
+        <v>95</v>
+      </c>
+      <c r="N3" s="12">
+        <v>28</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="17">
+        <v>9.2610416666666655</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>1000</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>127</v>
+      </c>
+      <c r="F4" s="12">
+        <v>118</v>
+      </c>
+      <c r="G4" s="12">
+        <v>115</v>
+      </c>
+      <c r="H4" s="12">
+        <v>111</v>
+      </c>
+      <c r="I4" s="12">
+        <v>102</v>
+      </c>
+      <c r="J4" s="12">
+        <v>81</v>
+      </c>
+      <c r="K4" s="12">
+        <v>87</v>
+      </c>
+      <c r="L4" s="12">
+        <v>90</v>
+      </c>
+      <c r="M4" s="12">
+        <v>80</v>
+      </c>
+      <c r="N4" s="12">
+        <v>89</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="17">
+        <v>9.9430555555555546</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>1000</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5">
+        <v>102</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6">
+        <v>148</v>
+      </c>
+      <c r="F5" s="6">
+        <v>98</v>
+      </c>
+      <c r="G5" s="6">
+        <v>85</v>
+      </c>
+      <c r="H5" s="6">
+        <v>74</v>
+      </c>
+      <c r="I5" s="7">
+        <v>76</v>
+      </c>
+      <c r="J5" s="7">
+        <v>85</v>
+      </c>
+      <c r="K5" s="6">
+        <v>87</v>
+      </c>
+      <c r="L5" s="6">
+        <v>70</v>
+      </c>
+      <c r="M5" s="6">
+        <v>55</v>
+      </c>
+      <c r="N5" s="6">
+        <v>60</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="17">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>838</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
+    <row r="6" spans="1:18">
+      <c r="A6" s="5">
+        <v>101</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6">
+        <v>104</v>
+      </c>
+      <c r="F6" s="6">
+        <v>78</v>
+      </c>
+      <c r="G6" s="6">
+        <v>77</v>
+      </c>
+      <c r="H6" s="6">
+        <v>72</v>
+      </c>
+      <c r="I6" s="7">
+        <v>69</v>
+      </c>
+      <c r="J6" s="8">
+        <v>70</v>
+      </c>
+      <c r="K6" s="6">
+        <v>70</v>
+      </c>
+      <c r="L6" s="6">
+        <v>71</v>
+      </c>
+      <c r="M6" s="6">
+        <v>69</v>
+      </c>
+      <c r="N6" s="6">
+        <v>74.649999999999977</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="17">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="11"/>
+      <c r="Q6" s="9">
+        <v>754.65</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="4">
+    <row r="7" spans="1:18">
+      <c r="A7" s="5">
         <v>100</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="6">
         <v>115</v>
       </c>
-      <c r="D3" s="5">
+      <c r="F7" s="6">
         <v>95</v>
       </c>
-      <c r="E3" s="5">
+      <c r="G7" s="6">
         <v>84</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H7" s="6">
         <v>80</v>
       </c>
-      <c r="G3" s="6">
+      <c r="I7" s="7">
         <v>70</v>
       </c>
-      <c r="H3" s="9">
+      <c r="J7" s="8">
         <v>63</v>
       </c>
-      <c r="I3" s="8">
+      <c r="K7" s="6">
         <v>64</v>
       </c>
-      <c r="J3" s="8">
+      <c r="L7" s="6">
         <v>59</v>
       </c>
-      <c r="K3" s="8">
+      <c r="M7" s="6">
         <v>57</v>
       </c>
-      <c r="L3" s="8">
+      <c r="N7" s="6">
         <v>56.450000000000045</v>
       </c>
-      <c r="M3" s="10">
+      <c r="O7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="17">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="9">
         <v>743.45</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="4">
-        <v>101</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5">
-        <v>104</v>
-      </c>
-      <c r="D4" s="5">
-        <v>78</v>
-      </c>
-      <c r="E4" s="5">
-        <v>77</v>
-      </c>
-      <c r="F4" s="5">
-        <v>72</v>
-      </c>
-      <c r="G4" s="6">
-        <v>69</v>
-      </c>
-      <c r="H4" s="9">
-        <v>70</v>
-      </c>
-      <c r="I4" s="8">
-        <v>70</v>
-      </c>
-      <c r="J4" s="8">
-        <v>71</v>
-      </c>
-      <c r="K4" s="8">
-        <v>69</v>
-      </c>
-      <c r="L4" s="8">
-        <v>74.649999999999977</v>
-      </c>
-      <c r="M4" s="10">
-        <v>754.65</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="4">
-        <v>102</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5">
-        <v>148</v>
-      </c>
-      <c r="D5" s="5">
-        <v>98</v>
-      </c>
-      <c r="E5" s="5">
-        <v>85</v>
-      </c>
-      <c r="F5" s="5">
-        <v>74</v>
-      </c>
-      <c r="G5" s="6">
-        <v>76</v>
-      </c>
-      <c r="H5" s="7">
-        <v>85</v>
-      </c>
-      <c r="I5" s="8">
-        <v>87</v>
-      </c>
-      <c r="J5" s="8">
-        <v>70</v>
-      </c>
-      <c r="K5" s="8">
-        <v>55</v>
-      </c>
-      <c r="L5" s="8">
-        <v>60</v>
-      </c>
-      <c r="M5" s="3">
-        <v>838</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>14</v>
+      <c r="R7" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -702,6 +931,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -714,6 +944,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>